<commit_message>
update web scraping notebooks
</commit_message>
<xml_diff>
--- a/IBM Data Science 25624/02- Web Scraping/wuzzuf.xlsx
+++ b/IBM Data Science 25624/02- Web Scraping/wuzzuf.xlsx
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Data Analyst Team Leader</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3Sixty</t>
+          <t>Confidential</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/HN6h2CLSlb04-Data-Analyst-Team-Leader-3Sixty-Giza-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/ewn4cDHL1bUW-Data-Analyst-Giza-Egypt</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,27 +500,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Business Data Analyst</t>
+          <t>Centro Data Program</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fawry Plus</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Smart Village, Giza, Egypt</t>
+          <t>Maadi, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/kvMsx40qvLZl-Business-Data-Analyst-Fawry-Plus-Giza-Egypt</t>
+          <t>https://wuzzuf.net/internship/j86RYZ2Qg0Wn-Centro-Data-Program-Centro-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Full Time</t>
+          <t>Internship</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -532,22 +532,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Big Data Consultant</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Exco Egypt</t>
+          <t>CRIF EGYPT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nasr City, Cairo, Egypt</t>
+          <t>Heliopolis, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/egjM6VMefvKW-Big-Data-Consultant-Exco-Egypt-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/AXcIDiTsKSWn-Data-Analyst-CRIF-EGYPT-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -564,54 +564,54 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Data/Business Analyst Intern</t>
+          <t>Data Analyst Team Leader</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>kafiil</t>
+          <t>3Sixty</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Maadi, Cairo, Egypt</t>
+          <t>Mohandessin, Giza, Egypt</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/internship/NXl1N6zwtmSd-DataBusiness-Analyst-Intern-kafiil-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/HN6h2CLSlb04-Data-Analyst-Team-Leader-3Sixty-Giza-Egypt</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Internship</t>
+          <t>Full Time</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>On-site</t>
+          <t>Hybrid</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Financial Data Analyst</t>
+          <t>Business Data Analyst</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Influence Communication</t>
+          <t>Fawry Plus</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Maadi, Cairo, Egypt</t>
+          <t>Smart Village, Giza, Egypt</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/pDJ6Rtkhmt6y-Financial-Data-Analyst-Influence-Communication-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/kvMsx40qvLZl-Business-Data-Analyst-Fawry-Plus-Giza-Egypt</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -628,22 +628,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Data Management Lead</t>
+          <t>Big Data Consultant</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BBI-Consultancy</t>
+          <t>Exco Egypt</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cairo, Egypt</t>
+          <t>Nasr City, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/KhhiGntCocD4-Data-Management-Lead-BBI-Consultancy-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/egjM6VMefvKW-Big-Data-Consultant-Exco-Egypt-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -660,12 +660,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Data Analytics Engineer</t>
+          <t>Data/Business Analyst Intern</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Erada</t>
+          <t>kafiil</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,12 +675,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/M0QOPoyJQ6Ia-Data-Analytics-Engineer-Erada-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/internship/NXl1N6zwtmSd-DataBusiness-Analyst-Intern-kafiil-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Full Time</t>
+          <t>Internship</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -692,22 +692,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BI &amp; Data Analytics Consultant</t>
+          <t>Financial Data Analyst</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mantrac</t>
+          <t>Influence Communication</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Alexandria, Egypt</t>
+          <t>Maadi, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/B2lwaYBkrVx3-BI-Data-Analytics-Consultant-Mantrac-Alexandria-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/pDJ6Rtkhmt6y-Financial-Data-Analyst-Influence-Communication-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -724,22 +724,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Data Management Lead</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Talaat Moustafa Group</t>
+          <t>BBI-Consultancy</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dokki, Giza, Egypt</t>
+          <t>Cairo, Egypt</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/n8eZCC5B0pgZ-Data-Analyst-Talaat-Moustafa-Group-Giza-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/KhhiGntCocD4-Data-Management-Lead-BBI-Consultancy-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -756,22 +756,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Data Analytics Engineer</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mazaya</t>
+          <t>Erada</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>New Cairo, Cairo, Egypt</t>
+          <t>Maadi, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/HaCk4dcFubh3-Data-Analyst-Mazaya-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/M0QOPoyJQ6Ia-Data-Analytics-Engineer-Erada-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -793,17 +793,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rotem SRS</t>
+          <t>Talaat Moustafa Group</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Cairo, Egypt</t>
+          <t>Dokki, Giza, Egypt</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/dZtsSzWqvAqg-Data-Analyst-Rotem-SRS-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/n8eZCC5B0pgZ-Data-Analyst-Talaat-Moustafa-Group-Giza-Egypt</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -820,22 +820,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>BI &amp; Data Analytics Consultant</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Al Watania Poultry</t>
+          <t>Mantrac</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Smart Village, Giza, Egypt</t>
+          <t>Alexandria, Egypt</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/HzJ6GhNp7osP-Data-Analyst-Al-Watania-Poultry-Giza-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/B2lwaYBkrVx3-BI-Data-Analytics-Consultant-Mantrac-Alexandria-Egypt</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -857,17 +857,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EGEC</t>
+          <t>Mazaya</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Haram, Giza, Egypt</t>
+          <t>New Cairo, Cairo, Egypt</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/F99QNVxDd8Yp-Data-Analyst-EGEC-Giza-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/HaCk4dcFubh3-Data-Analyst-Mazaya-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -884,22 +884,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Statistical analysis consultant</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Exco Egypt</t>
+          <t>Rotem SRS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Nasr City, Cairo, Egypt</t>
+          <t>Cairo, Egypt</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/SVlgFF15DPMx-Statistical-analysis-consultant-Exco-Egypt-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/dZtsSzWqvAqg-Data-Analyst-Rotem-SRS-Cairo-Egypt</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -921,17 +921,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alarabia Group</t>
+          <t>Al Watania Poultry</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cairo, Egypt</t>
+          <t>Smart Village, Giza, Egypt</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://wuzzuf.net/jobs/p/g31LAuLyaUXD-Data-Analyst-Alarabia-Group-Cairo-Egypt</t>
+          <t>https://wuzzuf.net/jobs/p/HzJ6GhNp7osP-Data-Analyst-Al-Watania-Poultry-Giza-Egypt</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">

</xml_diff>